<commit_message>
Added the Bank on the Tempate
I added the bank on the template, on the DebitOrderStatement,DebitOrder, PaymentData and
</commit_message>
<xml_diff>
--- a/Subs.Presentation/DOTemplate.xlsx
+++ b/Subs.Presentation/DOTemplate.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CSharp\Subs\Subs.Presentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nhlapot\Documents\GitHub\Subs\Subs.Presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C42E13-C591-4422-BEAA-3681A06FDBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F756987-CADA-47DE-8C30-0C83D750DA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{A19A4685-793F-4A57-85D3-04726907F1AD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A19A4685-793F-4A57-85D3-04726907F1AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="Datum">Sheet1!$A$2</definedName>
-    <definedName name="Items">Sheet1!$A$5:$AJ$5</definedName>
+    <definedName name="Items">Sheet1!$A$5:$AK$5</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>BInSol - U ver 1.00</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Data</t>
+  </si>
+  <si>
+    <t>BANK</t>
   </si>
 </sst>
 </file>
@@ -280,7 +283,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -458,6 +461,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -621,10 +630,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1000,33 +1013,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9057EA69-4BF8-4AAB-B448-111A0EF8A5AF}">
-  <dimension ref="A1:AJ160"/>
+  <dimension ref="A1:AK160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D160"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45413</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>62793076326</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1036,732 +1050,735 @@
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>6</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>7</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>8</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>9</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>10</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>11</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>12</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>13</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>14</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>15</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>17</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>18</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>19</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>20</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>21</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>22</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>23</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>24</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>25</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>26</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>27</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>28</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>29</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>30</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>31</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AG4" t="s">
         <v>32</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>33</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
         <v>34</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AJ4" t="s">
         <v>35</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AK4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="2"/>
-      <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
-      <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
-      <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
-      <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="2"/>
-      <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
-      <c r="D39" s="2"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
-      <c r="D40" s="2"/>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
-      <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" s="2"/>
-      <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43" s="2"/>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B44" s="2"/>
-      <c r="D44" s="2"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B45" s="2"/>
-      <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B46" s="2"/>
-      <c r="D46" s="2"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" s="2"/>
-      <c r="D47" s="2"/>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48" s="2"/>
-      <c r="D48" s="2"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="2"/>
-      <c r="D49" s="2"/>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50" s="2"/>
-      <c r="D50" s="2"/>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B51" s="2"/>
-      <c r="D51" s="2"/>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52" s="2"/>
-      <c r="D52" s="2"/>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53" s="2"/>
-      <c r="D53" s="2"/>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54" s="2"/>
-      <c r="D54" s="2"/>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B55" s="2"/>
-      <c r="D55" s="2"/>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B56" s="2"/>
-      <c r="D56" s="2"/>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="2"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B57" s="2"/>
-      <c r="D57" s="2"/>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="2"/>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B58" s="2"/>
-      <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B59" s="2"/>
-      <c r="D59" s="2"/>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B60" s="2"/>
-      <c r="D60" s="2"/>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="2"/>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B61" s="2"/>
-      <c r="D61" s="2"/>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="2"/>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B62" s="2"/>
-      <c r="D62" s="2"/>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E62" s="2"/>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B63" s="2"/>
-      <c r="D63" s="2"/>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E63" s="2"/>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B64" s="2"/>
-      <c r="D64" s="2"/>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B65" s="2"/>
-      <c r="D65" s="2"/>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E65" s="2"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B66" s="2"/>
-      <c r="D66" s="2"/>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="2"/>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B67" s="2"/>
-      <c r="D67" s="2"/>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E67" s="2"/>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B68" s="2"/>
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E68" s="2"/>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B69" s="2"/>
-      <c r="D69" s="2"/>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E69" s="2"/>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B70" s="2"/>
-      <c r="D70" s="2"/>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E70" s="2"/>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B71" s="2"/>
-      <c r="D71" s="2"/>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E71" s="2"/>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B72" s="2"/>
-      <c r="D72" s="2"/>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E72" s="2"/>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B73" s="2"/>
-      <c r="D73" s="2"/>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E73" s="2"/>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B74" s="2"/>
-      <c r="D74" s="2"/>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E74" s="2"/>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B75" s="2"/>
-      <c r="D75" s="2"/>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E75" s="2"/>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B76" s="2"/>
-      <c r="D76" s="2"/>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E76" s="2"/>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B77" s="2"/>
-      <c r="D77" s="2"/>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E77" s="2"/>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B78" s="2"/>
-      <c r="D78" s="2"/>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E78" s="2"/>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B79" s="2"/>
-      <c r="D79" s="2"/>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E79" s="2"/>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B80" s="2"/>
-      <c r="D80" s="2"/>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E80" s="2"/>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B81" s="2"/>
-      <c r="D81" s="2"/>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E81" s="2"/>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B82" s="2"/>
-      <c r="D82" s="2"/>
-    </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E82" s="2"/>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B83" s="2"/>
-      <c r="D83" s="2"/>
-    </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E83" s="2"/>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B84" s="2"/>
-      <c r="D84" s="2"/>
-    </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E84" s="2"/>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B85" s="2"/>
-      <c r="D85" s="2"/>
-    </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E85" s="2"/>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B86" s="2"/>
-      <c r="D86" s="2"/>
-    </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E86" s="2"/>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B87" s="2"/>
-      <c r="D87" s="2"/>
-    </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E87" s="2"/>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B88" s="2"/>
-      <c r="D88" s="2"/>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E88" s="2"/>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B89" s="2"/>
-      <c r="D89" s="2"/>
-    </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E89" s="2"/>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B90" s="2"/>
-      <c r="D90" s="2"/>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E90" s="2"/>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B91" s="2"/>
-      <c r="D91" s="2"/>
-    </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E91" s="2"/>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B92" s="2"/>
-      <c r="D92" s="2"/>
-    </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E92" s="2"/>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B93" s="2"/>
-      <c r="D93" s="2"/>
-    </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E93" s="2"/>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B94" s="2"/>
-      <c r="D94" s="2"/>
-    </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E94" s="2"/>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B95" s="2"/>
-      <c r="D95" s="2"/>
-    </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E95" s="2"/>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B96" s="2"/>
-      <c r="D96" s="2"/>
-    </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E96" s="2"/>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B97" s="2"/>
-      <c r="D97" s="2"/>
-    </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E97" s="2"/>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B98" s="2"/>
-      <c r="D98" s="2"/>
-    </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E98" s="2"/>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B99" s="2"/>
-      <c r="D99" s="2"/>
-    </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E99" s="2"/>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B100" s="2"/>
-      <c r="D100" s="2"/>
-    </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E100" s="2"/>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B101" s="2"/>
-      <c r="D101" s="2"/>
-    </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E101" s="2"/>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B102" s="2"/>
-      <c r="D102" s="2"/>
-    </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E102" s="2"/>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B103" s="2"/>
-      <c r="D103" s="2"/>
-    </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E103" s="2"/>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B104" s="2"/>
-      <c r="D104" s="2"/>
-    </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E104" s="2"/>
+    </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B105" s="2"/>
-      <c r="D105" s="2"/>
-    </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E105" s="2"/>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B106" s="2"/>
-      <c r="D106" s="2"/>
-    </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E106" s="2"/>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B107" s="2"/>
-      <c r="D107" s="2"/>
-    </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E107" s="2"/>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B108" s="2"/>
-      <c r="D108" s="2"/>
-    </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E108" s="2"/>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B109" s="2"/>
-      <c r="D109" s="2"/>
-    </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E109" s="2"/>
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B110" s="2"/>
-      <c r="D110" s="2"/>
-    </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E110" s="2"/>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B111" s="2"/>
-      <c r="D111" s="2"/>
-    </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E111" s="2"/>
+    </row>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B112" s="2"/>
-      <c r="D112" s="2"/>
-    </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E112" s="2"/>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B113" s="2"/>
-      <c r="D113" s="2"/>
-    </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E113" s="2"/>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B114" s="2"/>
-      <c r="D114" s="2"/>
-    </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E114" s="2"/>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B115" s="2"/>
-      <c r="D115" s="2"/>
-    </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E115" s="2"/>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B116" s="2"/>
-      <c r="D116" s="2"/>
-    </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E116" s="2"/>
+    </row>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B117" s="2"/>
-      <c r="D117" s="2"/>
-    </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E117" s="2"/>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B118" s="2"/>
-      <c r="D118" s="2"/>
-    </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E118" s="2"/>
+    </row>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B119" s="2"/>
-      <c r="D119" s="2"/>
-    </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E119" s="2"/>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B120" s="2"/>
-      <c r="D120" s="2"/>
-    </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E120" s="2"/>
+    </row>
+    <row r="121" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B121" s="2"/>
-      <c r="D121" s="2"/>
-    </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E121" s="2"/>
+    </row>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B122" s="2"/>
-      <c r="D122" s="2"/>
-    </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E122" s="2"/>
+    </row>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B123" s="2"/>
-      <c r="D123" s="2"/>
-    </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E123" s="2"/>
+    </row>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B124" s="2"/>
-      <c r="D124" s="2"/>
-    </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E124" s="2"/>
+    </row>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B125" s="2"/>
-      <c r="D125" s="2"/>
-    </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E125" s="2"/>
+    </row>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B126" s="2"/>
-      <c r="D126" s="2"/>
-    </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E126" s="2"/>
+    </row>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B127" s="2"/>
-      <c r="D127" s="2"/>
-    </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E127" s="2"/>
+    </row>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B128" s="2"/>
-      <c r="D128" s="2"/>
-    </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E128" s="2"/>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B129" s="2"/>
-      <c r="D129" s="2"/>
-    </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E129" s="2"/>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B130" s="2"/>
-      <c r="D130" s="2"/>
-    </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E130" s="2"/>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B131" s="2"/>
-      <c r="D131" s="2"/>
-    </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E131" s="2"/>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B132" s="2"/>
-      <c r="D132" s="2"/>
-    </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E132" s="2"/>
+    </row>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B133" s="2"/>
-      <c r="D133" s="2"/>
-    </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E133" s="2"/>
+    </row>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B134" s="2"/>
-      <c r="D134" s="2"/>
-    </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E134" s="2"/>
+    </row>
+    <row r="135" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B135" s="2"/>
-      <c r="D135" s="2"/>
-    </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E135" s="2"/>
+    </row>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B136" s="2"/>
-      <c r="D136" s="2"/>
-    </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E136" s="2"/>
+    </row>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B137" s="2"/>
-      <c r="D137" s="2"/>
-    </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E137" s="2"/>
+    </row>
+    <row r="138" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B138" s="2"/>
-      <c r="D138" s="2"/>
-    </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E138" s="2"/>
+    </row>
+    <row r="139" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B139" s="2"/>
-      <c r="D139" s="2"/>
-    </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E139" s="2"/>
+    </row>
+    <row r="140" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B140" s="2"/>
-      <c r="D140" s="2"/>
-    </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E140" s="2"/>
+    </row>
+    <row r="141" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B141" s="2"/>
-      <c r="D141" s="2"/>
-    </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E141" s="2"/>
+    </row>
+    <row r="142" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B142" s="2"/>
-      <c r="D142" s="2"/>
-    </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E142" s="2"/>
+    </row>
+    <row r="143" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B143" s="2"/>
-      <c r="D143" s="2"/>
-    </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E143" s="2"/>
+    </row>
+    <row r="144" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B144" s="2"/>
-      <c r="D144" s="2"/>
-    </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E144" s="2"/>
+    </row>
+    <row r="145" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B145" s="2"/>
-      <c r="D145" s="2"/>
-    </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E145" s="2"/>
+    </row>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B146" s="2"/>
-      <c r="D146" s="2"/>
-    </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E146" s="2"/>
+    </row>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B147" s="2"/>
-      <c r="D147" s="2"/>
-    </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E147" s="2"/>
+    </row>
+    <row r="148" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B148" s="2"/>
-      <c r="D148" s="2"/>
-    </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E148" s="2"/>
+    </row>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B149" s="2"/>
-      <c r="D149" s="2"/>
-    </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E149" s="2"/>
+    </row>
+    <row r="150" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B150" s="2"/>
-      <c r="D150" s="2"/>
-    </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E150" s="2"/>
+    </row>
+    <row r="151" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B151" s="2"/>
-      <c r="D151" s="2"/>
-    </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E151" s="2"/>
+    </row>
+    <row r="152" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B152" s="2"/>
-      <c r="D152" s="2"/>
-    </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E152" s="2"/>
+    </row>
+    <row r="153" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B153" s="2"/>
-      <c r="D153" s="2"/>
-    </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E153" s="2"/>
+    </row>
+    <row r="154" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B154" s="2"/>
-      <c r="D154" s="2"/>
-    </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E154" s="2"/>
+    </row>
+    <row r="155" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B155" s="2"/>
-      <c r="D155" s="2"/>
-    </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E155" s="2"/>
+    </row>
+    <row r="156" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B156" s="2"/>
-      <c r="D156" s="2"/>
-    </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E156" s="2"/>
+    </row>
+    <row r="157" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B157" s="2"/>
-      <c r="D157" s="2"/>
-    </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E157" s="2"/>
+    </row>
+    <row r="158" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B158" s="2"/>
-      <c r="D158" s="2"/>
-    </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E158" s="2"/>
+    </row>
+    <row r="159" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B159" s="2"/>
-      <c r="D159" s="2"/>
-    </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E159" s="2"/>
+    </row>
+    <row r="160" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B160" s="2"/>
-      <c r="D160" s="2"/>
+      <c r="E160" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>